<commit_message>
Quickdrive consists ZWNL 2022
</commit_message>
<xml_diff>
--- a/hvnl-2022.xlsx
+++ b/hvnl-2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{357FA9F9-7B12-4D5F-8FF7-450A1A36A9F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97FEB55A-9F9D-47C2-BAC4-EDB531C5CF29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23077" yWindow="4838" windowWidth="21503" windowHeight="12975" xr2:uid="{F5835F28-5191-4B2A-BC18-5C599A3AF286}"/>
+    <workbookView xWindow="0" yWindow="2625" windowWidth="21503" windowHeight="12975" xr2:uid="{F5835F28-5191-4B2A-BC18-5C599A3AF286}"/>
   </bookViews>
   <sheets>
     <sheet name="Standard" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B14" authorId="0" shapeId="0" xr:uid="{6FF0DA75-8C84-44C2-BC2F-A5AD6D7614D4}">
+    <comment ref="B15" authorId="0" shapeId="0" xr:uid="{6FF0DA75-8C84-44C2-BC2F-A5AD6D7614D4}">
       <text>
         <r>
           <rPr>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>Naam</t>
   </si>
@@ -171,6 +171,59 @@
   </si>
   <si>
     <t>nvt</t>
+  </si>
+  <si>
+    <t>7322 Rhn-Bkl</t>
+  </si>
+  <si>
+    <t>Rhn-Db:
+- 7323
+- 3022*
+- 3125
+- 7325</t>
+  </si>
+  <si>
+    <t>Db-Ut:
+- 7425
+- 105
+- 3225
+- 6027
+- 3127
+- 3927 rijdt niet
+- 3924* rijdt niet
+- 7327</t>
+  </si>
+  <si>
+    <t>Ut-Bkl:
+- 7427
+- 3027
+- 3227
+- 829
+- 3129
+- 3124*</t>
+  </si>
+  <si>
+    <t>Ut:
+- 527
+- 622
+- 2029
+- 3124*
+- 3527
+- 5725/4926
+- 5622/5627
+- 6024/8824
+- 6929</t>
+  </si>
+  <si>
+    <t>- Klmos Mrg
+- Kalk/staaltrein Bnk 0907</t>
+  </si>
+  <si>
+    <t>Bkl: geen</t>
+  </si>
+  <si>
+    <t>- Utoz
+- Ut noord</t>
   </si>
 </sst>
 </file>
@@ -237,7 +290,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -250,6 +303,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -564,138 +624,181 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B67FE5B9-9D71-4D65-AFBF-5E94D529D4E1}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="18.33203125" customWidth="1"/>
     <col min="2" max="2" width="26.46484375" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="199.5" x14ac:dyDescent="0.45">
+      <c r="C2" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="199.5" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C3" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="128.25" x14ac:dyDescent="0.45">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C4" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="142.5" x14ac:dyDescent="0.45">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C5" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C6" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C7" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C8" s="8"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A10" s="1" t="s">
+      <c r="C9" s="8"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A10" s="1"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="8"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A11" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C11" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B13" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A13" s="1" t="s">
+      <c r="C13" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A14" s="1" t="s">
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A15" s="1" t="s">
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A16" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A20" s="1" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C3:C10">
+    <sortCondition ref="C3:C10"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>

</xml_diff>